<commit_message>
ya esta ingresos en flujo de caja
</commit_message>
<xml_diff>
--- a/backend/src/tmp/37.xlsx
+++ b/backend/src/tmp/37.xlsx
@@ -11,24 +11,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Ingresos(*)</t>
   </si>
   <si>
-    <t>Ingreso 1</t>
-  </si>
-  <si>
-    <t>Ingreso 2</t>
-  </si>
-  <si>
-    <t>Ingreso 3</t>
-  </si>
-  <si>
-    <t>Ingreso 4</t>
-  </si>
-  <si>
-    <t>Ingreso 5</t>
+    <t>Prestamo</t>
+  </si>
+  <si>
+    <t>Donaciones</t>
+  </si>
+  <si>
+    <t>Patrocinador</t>
+  </si>
+  <si>
+    <t>Pago Cliente</t>
+  </si>
+  <si>
+    <t>Total Ingresos</t>
   </si>
   <si>
     <t>Egresos</t>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>Egreso 4</t>
+  </si>
+  <si>
+    <t>Total Egresos</t>
+  </si>
+  <si>
+    <t>Acumulado</t>
   </si>
 </sst>
 </file>
@@ -59,15 +65,20 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -75,12 +86,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,60 +447,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="4" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>69133</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>89841</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>100056</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>80801</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>59980</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>59980</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>309970</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -481,7 +542,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -489,7 +550,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -497,7 +558,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -505,12 +566,28 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>180000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>NaN</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya estan los reportes
</commit_message>
<xml_diff>
--- a/backend/src/tmp/37.xlsx
+++ b/backend/src/tmp/37.xlsx
@@ -31,7 +31,7 @@
     <t>Total Ingresos</t>
   </si>
   <si>
-    <t>Egresos</t>
+    <t>Egresos(*)</t>
   </si>
   <si>
     <t>Egreso 1</t>
@@ -539,7 +539,13 @@
         <v>7</v>
       </c>
       <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>10000</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -547,7 +553,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>40000</v>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>20000</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,7 +567,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>90000</v>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>30000</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,7 +581,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>80000</v>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>40000</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,7 +595,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>180000</v>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>60000</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -579,7 +609,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>400000</v>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>160000</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>